<commit_message>
updated input data (including graphs for SI)
</commit_message>
<xml_diff>
--- a/code/COSA_Data/historical_feed-in_tariff.xlsx
+++ b/code/COSA_Data/historical_feed-in_tariff.xlsx
@@ -6126,6 +6126,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6962,6 +6963,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9199,8 +9201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ944"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT4" workbookViewId="0">
-      <selection activeCell="BH10" sqref="BH10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>